<commit_message>
Formatted indices of fit tables
</commit_message>
<xml_diff>
--- a/Datasets/StatisticalTables/Indices of fit for all models.xlsx
+++ b/Datasets/StatisticalTables/Indices of fit for all models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdullahiqbal/Desktop/Documents/Dat5902FinalProject/dat5902Project/Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdullahiqbal/Desktop/Documents/Dat5902FinalProject/dat5902Project/Datasets/StatisticalTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02013C3-DD7B-F44C-A0B6-3C9A1854EC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FD379C-A1F0-B44A-8608-A5EA154CA4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5060" windowWidth="27640" windowHeight="16940" xr2:uid="{22075999-EF60-EE4E-8665-74046C2C998A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Value</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>chi2 p-value</t>
+  </si>
+  <si>
+    <t>Hypothesis Model</t>
+  </si>
+  <si>
+    <t>Final Model</t>
   </si>
 </sst>
 </file>
@@ -116,9 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A7E986-63E9-9D40-BF3C-24B8B52FCE0F}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A2:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:O2"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,280 +473,231 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>8</v>
-      </c>
-      <c r="D2">
+      <c r="D4">
         <v>48.655132999999999</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E4" s="1">
         <v>2.6102179999999999E-9</v>
       </c>
-      <c r="F2">
+      <c r="F4">
         <v>98.099002999999996</v>
       </c>
-      <c r="G2">
+      <c r="G4">
         <v>0.51547600000000005</v>
       </c>
-      <c r="H2">
+      <c r="H4">
         <v>0.50402000000000002</v>
       </c>
-      <c r="I2">
+      <c r="I4">
+        <v>0.22476199999999999</v>
+      </c>
+      <c r="J4">
+        <v>0.32831500000000002</v>
+      </c>
+      <c r="K4">
+        <v>8.8132889999999993</v>
+      </c>
+      <c r="L4">
+        <v>20.846886000000001</v>
+      </c>
+      <c r="M4">
+        <v>0.59335499999999997</v>
+      </c>
+      <c r="N4">
         <v>0.206432</v>
       </c>
-      <c r="J2">
+      <c r="O4">
         <v>0.50402000000000002</v>
-      </c>
-      <c r="K2">
-        <v>0.22476199999999999</v>
-      </c>
-      <c r="L2">
-        <v>0.32831500000000002</v>
-      </c>
-      <c r="M2">
-        <v>8.8132889999999993</v>
-      </c>
-      <c r="N2">
-        <v>20.846886000000001</v>
-      </c>
-      <c r="O2">
-        <v>0.59335499999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" t="s">
         <v>7</v>
-      </c>
-      <c r="D7">
-        <v>10.38003</v>
-      </c>
-      <c r="E7">
-        <v>3.449E-2</v>
-      </c>
-      <c r="F7">
-        <v>152.00415100000001</v>
-      </c>
-      <c r="G7">
-        <v>0.95600099999999999</v>
-      </c>
-      <c r="H7">
-        <v>0.93171199999999998</v>
-      </c>
-      <c r="I7">
-        <v>0.88049599999999995</v>
-      </c>
-      <c r="J7">
-        <v>0.93171199999999998</v>
-      </c>
-      <c r="K7">
-        <v>0.92300199999999999</v>
-      </c>
-      <c r="L7">
-        <v>0.14032600000000001</v>
-      </c>
-      <c r="M7">
-        <v>11.746829</v>
-      </c>
-      <c r="N7">
-        <v>26.187144</v>
-      </c>
-      <c r="O7">
-        <v>0.126586</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="C9">
         <v>7</v>
       </c>
-      <c r="K9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" t="s">
-        <v>10</v>
-      </c>
-      <c r="N9" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>7</v>
-      </c>
-      <c r="D10">
+      <c r="D9">
         <v>7.262365</v>
       </c>
-      <c r="E10">
+      <c r="E9">
         <v>6.3989000000000004E-2</v>
       </c>
-      <c r="F10">
+      <c r="F9">
         <v>100.60639</v>
       </c>
-      <c r="G10">
+      <c r="G9">
         <v>0.95446500000000001</v>
       </c>
-      <c r="H10">
+      <c r="H9">
         <v>0.92781400000000003</v>
       </c>
-      <c r="I10">
+      <c r="I9">
+        <v>0.89375199999999999</v>
+      </c>
+      <c r="J9">
+        <v>0.132441</v>
+      </c>
+      <c r="K9">
+        <v>13.822869000000001</v>
+      </c>
+      <c r="L9">
+        <v>30.669903999999999</v>
+      </c>
+      <c r="M9">
+        <v>8.8565000000000005E-2</v>
+      </c>
+      <c r="N9">
         <v>0.83156600000000003</v>
       </c>
-      <c r="J10">
+      <c r="O9">
         <v>0.92781400000000003</v>
-      </c>
-      <c r="K10">
-        <v>0.89375199999999999</v>
-      </c>
-      <c r="L10">
-        <v>0.132441</v>
-      </c>
-      <c r="M10">
-        <v>13.822869000000001</v>
-      </c>
-      <c r="N10">
-        <v>30.669903999999999</v>
-      </c>
-      <c r="O10">
-        <v>8.8565000000000005E-2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A7:O7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>